<commit_message>
cleaning v1 after stable v1
</commit_message>
<xml_diff>
--- a/data/Synonyms.xlsx
+++ b/data/Synonyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khalid.khader\Desktop\Work\Medical_Prescription_Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521CFA26-ED96-4E2B-8F30-BF161E20D630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0D1760-FB3A-4065-A170-7810395A2ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="1158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="1160">
   <si>
     <t>hicl_seqno</t>
   </si>
@@ -3510,6 +3510,12 @@
   </si>
   <si>
     <t>Cefprozil</t>
+  </si>
+  <si>
+    <t>Amoxicillin</t>
+  </si>
+  <si>
+    <t>Amoxil</t>
   </si>
 </sst>
 </file>
@@ -3994,10 +4000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C670"/>
+  <dimension ref="A1:C671"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B653" workbookViewId="0">
-      <selection activeCell="C674" sqref="C674"/>
+    <sheetView tabSelected="1" topLeftCell="B657" workbookViewId="0">
+      <selection activeCell="C673" sqref="C673"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11374,6 +11380,14 @@
         <v>1157</v>
       </c>
     </row>
+    <row r="671" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B671" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C671" s="2" t="s">
+        <v>1159</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C669">
     <sortCondition ref="B2:B669"/>

</xml_diff>